<commit_message>
Added Not Specified note if good for how many people is empty in the Excel file
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>THE ONES RESTAURANT MENU</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>₱350.00</t>
+  </si>
+  <si>
+    <t>Not specified</t>
   </si>
   <si>
     <t>Grilled Veggies with Chicken</t>
@@ -763,32 +766,32 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="13.68" customHeight="true">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="41.04" customHeight="true">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -797,398 +800,398 @@
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="41.04" customHeight="true">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" ht="27.36" customHeight="true">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="13.68" customHeight="true">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="9" ht="41.04" customHeight="true">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="10" ht="13.68" customHeight="true">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="11" ht="27.36" customHeight="true">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="12" ht="13.68" customHeight="true">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" ht="41.04" customHeight="true">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="14" ht="27.36" customHeight="true">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" ht="27.36" customHeight="true">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="16" ht="27.36" customHeight="true">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" ht="27.36" customHeight="true">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="18" ht="27.36" customHeight="true">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" ht="27.36" customHeight="true">
       <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" ht="27.36" customHeight="true">
       <c r="A20" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="21" ht="82.08" customHeight="true">
       <c r="A21" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.68" customHeight="true">
       <c r="A22" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="23" ht="13.68" customHeight="true">
       <c r="A23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="24" ht="13.68" customHeight="true">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="25" ht="13.68" customHeight="true">
       <c r="A25" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v/>
+        <v>10</v>
       </c>
     </row>
     <row r="26" ht="27.36" customHeight="true">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" ht="27.36" customHeight="true">
       <c r="A27" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" ht="27.36" customHeight="true">
       <c r="A28" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 new items in Meal Category
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>THE ONES RESTAURANT MENU</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Sinugba Porkchop Bangs and Chicken</t>
+  </si>
+  <si>
+    <t>Sinugba is a type of barbecue that is cooked on a grill over charcoal and paired with chicken.</t>
+  </si>
+  <si>
+    <t>₱700.00</t>
+  </si>
+  <si>
+    <t>Pork Afritada</t>
+  </si>
+  <si>
+    <t>Pork Afritada is a Filipino pork stew that is composed of pork slices along with hotdog, potato and carrot.</t>
   </si>
   <si>
     <t>Calamares (Big Size)</t>
@@ -691,7 +706,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -998,10 +1013,10 @@
         <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -1015,30 +1030,30 @@
         <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" ht="27.36" customHeight="true">
       <c r="A19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" ht="27.36" customHeight="true">
@@ -1049,16 +1064,16 @@
         <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" ht="82.08" customHeight="true">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" ht="27.36" customHeight="true">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1066,44 +1081,44 @@
         <v>61</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" ht="27.36" customHeight="true">
+      <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" ht="13.68" customHeight="true">
-      <c r="A22" s="3" t="s">
+      <c r="C22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" ht="82.08" customHeight="true">
+      <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" ht="13.68" customHeight="true">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>10</v>
@@ -1117,7 +1132,7 @@
         <v>70</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>37</v>
@@ -1128,13 +1143,13 @@
     </row>
     <row r="25" ht="13.68" customHeight="true">
       <c r="A25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>37</v>
@@ -1143,55 +1158,89 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" ht="27.36" customHeight="true">
+    <row r="26" ht="13.68" customHeight="true">
       <c r="A26" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" ht="13.68" customHeight="true">
+      <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" ht="27.36" customHeight="true">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" ht="27.36" customHeight="true">
       <c r="A28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="29" ht="27.36" customHeight="true">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" ht="27.36" customHeight="true">
+      <c r="A30" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>